<commit_message>
Update: BoM list, Docs
</commit_message>
<xml_diff>
--- a/HW/Product/BoM/THEGIOIIC.xlsx
+++ b/HW/Product/BoM/THEGIOIIC.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\SAMPI\P16DK\P16F1887x\HW\Product\BoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD49327D-BDBE-43EB-B8DF-AD7F29716AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B361B0-EA1D-4E9B-95AC-B83423A89ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="507" xr2:uid="{AC2C9739-183B-4393-85EE-4EA8A3EEC5E3}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="507" xr2:uid="{AC2C9739-183B-4393-85EE-4EA8A3EEC5E3}"/>
   </bookViews>
   <sheets>
     <sheet name="VN" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -320,7 +322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +381,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -417,7 +427,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,6 +484,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -801,7 +829,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +846,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" s="3">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -862,10 +890,10 @@
       </c>
       <c r="F3" s="16">
         <f t="shared" ref="F3:F31" si="0">F$1*E3</f>
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="G3" s="17">
-        <v>100</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -886,34 +914,34 @@
       </c>
       <c r="F4" s="16">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>176</v>
       </c>
       <c r="G4" s="17">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="24">
         <v>2</v>
       </c>
-      <c r="F5" s="16">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="F5" s="17">
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="G5" s="17">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -934,10 +962,10 @@
       </c>
       <c r="F6" s="16">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="G6" s="17">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -958,10 +986,10 @@
       </c>
       <c r="F7" s="16">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G7" s="17">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -982,34 +1010,34 @@
       </c>
       <c r="F8" s="16">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G8" s="17">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="9" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="24">
         <v>3</v>
       </c>
-      <c r="F9" s="16">
-        <f t="shared" si="0"/>
-        <v>48</v>
+      <c r="F9" s="17">
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="G9" s="17">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,154 +1058,154 @@
       </c>
       <c r="F10" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G10" s="17">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="24">
         <v>2</v>
       </c>
-      <c r="F11" s="16">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="F11" s="17">
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="G11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>10</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="24">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>11</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="C13" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>12</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="24">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>13</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="24">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>14</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="15">
-        <v>1</v>
-      </c>
-      <c r="F12" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G12" s="17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>11</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="15">
-        <v>1</v>
-      </c>
-      <c r="F13" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G13" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>12</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="15">
-        <v>1</v>
-      </c>
-      <c r="F14" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G14" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>13</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="G15" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
-        <v>14</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="15">
-        <v>1</v>
-      </c>
-      <c r="F16" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="E16" s="24">
+        <v>1</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="G16" s="17">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1198,10 +1226,10 @@
       </c>
       <c r="F17" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G17" s="17">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1222,10 +1250,10 @@
       </c>
       <c r="F18" s="16">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G18" s="17">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1246,10 +1274,10 @@
       </c>
       <c r="F19" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G19" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1270,10 +1298,10 @@
       </c>
       <c r="F20" s="16">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G20" s="17">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1294,10 +1322,10 @@
       </c>
       <c r="F21" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G21" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1318,10 +1346,10 @@
       </c>
       <c r="F22" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G22" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1342,10 +1370,10 @@
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G23" s="17">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1366,10 +1394,10 @@
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G24" s="17">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1390,10 +1418,10 @@
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G25" s="17">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1414,10 +1442,10 @@
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G26" s="17">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1438,34 +1466,34 @@
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G27" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
         <v>26</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="15">
-        <v>1</v>
-      </c>
-      <c r="F28" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="G28" s="17">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1486,10 +1514,10 @@
       </c>
       <c r="F29" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G29" s="17">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1510,10 +1538,10 @@
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G30" s="17">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1534,10 +1562,10 @@
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G31" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>